<commit_message>
creating usefull function notebook
</commit_message>
<xml_diff>
--- a/Sentences/corrected_sentences_with_LPC.xlsx
+++ b/Sentences/corrected_sentences_with_LPC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/hagars1_mail_tau_ac_il/Documents/Desktop/Stage/LPC_2022/Sentences/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hita/Dropbox/LPC/LPC EEG and eye tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA194683-A541-43B7-9AA5-14C0B9285C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA49F81-3EBE-5F43-AA7B-8D1AB5B91CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="corrected_sentences_with_LPC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Predictable end sentence</t>
   </si>
@@ -64,7 +64,7 @@
     <t>Les jours ensoleillés, Jacques se rend au parc pour promener son chien.</t>
   </si>
   <si>
-    <t>Pendant les grandes vacances, le médecin allait marcher avec son chien.</t>
+    <t>Pendant les grandes vacances, le médecin aimait voyager avec son chien.</t>
   </si>
   <si>
     <t>chien</t>
@@ -73,16 +73,16 @@
     <t>24, check the cv for: {'les': 1, 'ensoleillés': 4, 'pour': 2, 'son': 1}</t>
   </si>
   <si>
-    <t>24, check the cv for: {'pendant': 2, 'les': 1, 'grandes': 3, 'le': 1, 'son': 1}</t>
+    <t>25, check the cv for: {'pendant': 2, 'les': 1, 'grandes': 3, 'le': 1, 'son': 1}</t>
   </si>
   <si>
     <t>le   Zu-R   @-so-lE-je   Za-k   s2   R@   o   pa-R-k   pu-R   p-RO-m-ne   s§   S-j5   ,check the cv for: {'les': 'le', 'ensoleillés': '@solEje', 'pour': 'puR', 'son': 's§'}</t>
   </si>
   <si>
-    <t>p@-d@   le   g-R@-d   va-k@-s   l2   mE-d-s5   a-lE   ma-R-Se   a-vE-k   s§   S-j5   ,check the cv for: {'pendant': 'p@d@', 'les': 'le', 'grandes': 'gR@d', 'le': 'l2', 'son': 's§'}</t>
-  </si>
-  <si>
-    <t>Émilie l’avait détesté dès le moment où elles s'étaient rencontrées.</t>
+    <t>p@-d@   le   g-R@-d   va-k@-s   l2   mE-d-s5   E-mE   v-wa-ja-Ze   a-vE-k   s§   S-j5   ,check the cv for: {'pendant': 'p@d@', 'les': 'le', 'grandes': 'gR@d', 'le': 'l2', 'son': 's§'}</t>
+  </si>
+  <si>
+    <t>Émilie l’avait détestée dès le moment où elles s'étaient rencontrées.</t>
   </si>
   <si>
     <t>Les policiers n'avaient pas du tout compris qu'elles s'étaient rencontrées</t>
@@ -91,79 +91,52 @@
     <t>rencontrées</t>
   </si>
   <si>
-    <t>15, except ['émilie', 'l’avait', "s'étaient"], check the cv for: {'détesté': 4, 'le': 1, 'où': 1, 'rencontrées': 4}</t>
+    <t>15, except ['émilie', 'l’avait', "s'étaient"], check the cv for: {'détestée': 4, 'le': 1, 'où': 1, 'rencontrées': 4}</t>
   </si>
   <si>
     <t>15, except ["n'avaient", "qu'elles", "s'étaient"], check the cv for: {'les': 1, 'policiers': 4, 'pas': 1, 'tout': 1, 'compris': 3, 'rencontrées': 4}</t>
   </si>
   <si>
-    <t>de-tE-s-te   dE   l2   mo-m@   u   E-l   R@-k§-t-Re   ,except ['émilie', 'l’avait', "s'étaient"], check the phon for: {'détesté': 'detEste', 'le': 'l2', 'où': 'u', 'rencontrées': 'R@k§tRe'}</t>
+    <t>de-tE-s-te   dE   l2   mo-m@   u   E-l   R@-k§-t-Re   ,except ['émilie', 'l’avait', "s'étaient"], check the phon for: {'détestée': 'detEste', 'le': 'l2', 'où': 'u', 'rencontrées': 'R@k§tRe'}</t>
   </si>
   <si>
     <t>le   po-li-s-je   pa   dy   tu   k§-p-Ri   R@-k§-t-Re   ,except ["n'avaient", "qu'elles", "s'étaient"], check the phon for: {'les': 'le', 'policiers': 'polisje', 'pas': 'pa', 'tout': 'tu', 'compris': 'k§pRi', 'rencontrées': 'R@k§tRe'}</t>
   </si>
   <si>
-    <t>Cette chemise est trop vieille, sa matière est vraiment usée.</t>
-  </si>
-  <si>
-    <t>Pour se réchauffer, il a mis une couverture très usée.</t>
-  </si>
-  <si>
-    <t>usée</t>
-  </si>
-  <si>
-    <t>19, except ['chemise'], check the cv for: {'est': 1, 'vieille': 3, 'sa': 1, 'usée': 2}</t>
-  </si>
-  <si>
-    <t>21, check the cv for: {'pour': 2, 'il': 2, 'a': 1, 'mis': 1, 'une': 2, 'usée': 2}</t>
-  </si>
-  <si>
-    <t>sE-t   e   t-Ro   v-jE-j   sa   ma-t-jE-R   e   v-RE-m@   y-ze   ,except ['chemise'], check the phon for: {'est': 'e', 'vieille': 'vjEj', 'sa': 'sa', 'usée': 'yze'}</t>
-  </si>
-  <si>
-    <t>pu-R   s2   Re-So-fe   i-l   a   mi   y-n   ku-vE-R-ty-R   t-RE   y-ze   ,check the cv for: {'pour': 'puR', 'il': 'il', 'a': 'a', 'mis': 'mi', 'une': 'yn', 'usée': 'yze'}</t>
-  </si>
-  <si>
-    <t>Le petit oiseau s'est cassé une aile et ne peut plus voler.</t>
-  </si>
-  <si>
-    <t>Les deux anges pensaient à leur avenir et s'entrainaient à voler.</t>
-  </si>
-  <si>
-    <t>voler</t>
-  </si>
-  <si>
-    <t>19 check the cv for: {'le': 1, 'cassé': 2, 'une': 2, 'plus': 2}</t>
-  </si>
-  <si>
-    <t>20 check the cv for: {'les': 1, 'leur': 2}</t>
-  </si>
-  <si>
-    <t>l2   wa-zo   ka-se   y-n   E-l   e   n2   p2   p-ly   vo-le   ,except ['petit', "s'est"], check the phon for: {'le': 'l2', 'cassé': 'kase', 'une': 'yn', 'plus': 'ply'}</t>
-  </si>
-  <si>
-    <t>le   d2   @-Z   p@-sE   a   l9-R   e   a   vo-le   ,except ['avenir', "s'entrainaient"], check the phon for: {'les': 'le', 'leur': 'l9R'}</t>
-  </si>
-  <si>
-    <t>Le magicien a fait tomber le rideau et la femme avait disparu.</t>
-  </si>
-  <si>
-    <t>les hommes voulaient voir le maire mais il avait encore disparu.</t>
+    <t>Cette jupe est trop vieille, son tissu est très usé.</t>
+  </si>
+  <si>
+    <t>Pour se réchauffer, il a mis un manteau très usé.</t>
+  </si>
+  <si>
+    <t>18, check the cv for: {'est': 1, 'vieille': 3, 'son': 1, 'tissu': 2, 'usé': 2}</t>
+  </si>
+  <si>
+    <t>17, check the cv for: {'pour': 2, 'il': 2, 'a': 1, 'mis': 1, 'un': 1, 'usé': 2}</t>
+  </si>
+  <si>
+    <t>sE-t   Zy-p   e   t-Ro   v-jE-j   s§   ti-sy   e   t-RE   y-ze   ,check the cv for: {'est': 'e', 'vieille': 'vjEj', 'son': 's§', 'tissu': 'tisy', 'usé': 'yze'}</t>
+  </si>
+  <si>
+    <t>pu-R   s2   Re-So-fe   i-l   a   mi   1   m@-to   t-RE   y-ze   ,check the cv for: {'pour': 'puR', 'il': 'il', 'a': 'a', 'mis': 'mi', 'un': '1', 'usé': 'yze'}</t>
+  </si>
+  <si>
+    <t>Le magicien fit tomber le rideau et la femme avait disparu.</t>
   </si>
   <si>
     <t>disparu</t>
   </si>
   <si>
-    <t>22, check the cv for: {'le': 1, 'a': 1, 'fait': 1, 'la': 1, 'avait': 2, 'disparu': 4}</t>
-  </si>
-  <si>
-    <t>23, check the cv for: {'les': 1, 'le': 1, 'mais': 1, 'il': 2, 'avait': 2, 'disparu': 4}</t>
-  </si>
-  <si>
-    <t>l2   ma-Zi-s-j5   a   fE   t§-be   l2   Ri-do   e   la   fa-m   a-vE   di-s-pa-Ry   ,check the cv for: {'le': 'l2', 'a': 'a', 'fait': 'fE', 'la': 'la', 'avait': 'avE', 'disparu': 'dispaRy'}</t>
-  </si>
-  <si>
-    <t>le   O-m   vu-lE   v-wa-R   l2   mE-R   mE   i-l   a-vE   @-kO-R   di-s-pa-Ry   ,check the cv for: {'les': 'le', 'le': 'l2', 'mais': 'mE', 'il': 'il', 'avait': 'avE', 'disparu': 'dispaRy'}</t>
+    <t>21, check the cv for: {'le': 1, 'la': 1, 'avait': 2, 'disparu': 4}</t>
+  </si>
+  <si>
+    <t>21, except ["qu'il"], check the cv for: {'les': 1, 'le': 1, 'avait': 2, 'disparu': 4}</t>
+  </si>
+  <si>
+    <t>l2   ma-Zi-s-j5   fi   t§-be   l2   Ri-do   e   la   fa-m   a-vE   di-s-pa-Ry   ,check the cv for: {'le': 'l2', 'la': 'la', 'avait': 'avE', 'disparu': 'dispaRy'}</t>
+  </si>
+  <si>
+    <t>le   vi-zi-t9-R   a-t@-dE   l2   mE-R   e   i-No-RE   a-vE   di-s-pa-Ry   ,except ["qu'il"], check the phon for: {'les': 'le', 'le': 'l2', 'avait': 'avE', 'disparu': 'dispaRy'}</t>
   </si>
   <si>
     <t>Il voulait travailler pour mon entreprise et n'a pas hésité à signer le contrat.</t>
@@ -250,52 +223,43 @@
     <t>la   fa-m   o-fE-R   1   bo   d2   pE-R-l   ,except ['s’était', 'bracelet'], check the phon for: {'la': 'la', 'un': '1', 'beau': 'bo', 'de': 'd2'}</t>
   </si>
   <si>
-    <t>Pour atténuer l’amertume de son café, elle a mis un morceau de sucre.</t>
-  </si>
-  <si>
-    <t>Pour améliorer cette recette, il faudrait ajouter un peu plus de sucre.</t>
+    <t>Pour rendre son café moins amer, elle a mis un morceau de sucre.</t>
   </si>
   <si>
     <t>sucre</t>
   </si>
   <si>
-    <t>22, except ['l’amertume'], check the cv for: {'pour': 2, 'de': 1, 'son': 1, 'café': 2, 'a': 1, 'mis': 1, 'un': 1, 'sucre': 3}</t>
+    <t>25, check the cv for: {'pour': 2, 'son': 1, 'café': 2, 'moins': 2, 'amer': 3, 'a': 1, 'mis': 1, 'un': 1, 'de': 1, 'sucre': 3}</t>
   </si>
   <si>
     <t>25, except ['recette'], check the cv for: {'pour': 2, 'il': 2, 'un': 1, 'peu': 1, 'plus': 2, 'de': 1, 'sucre': 3}</t>
   </si>
   <si>
-    <t>pu-R   a-te-n-8e   d2   s§   ka-fe   E-l   a   mi   1   mO-R-so   d2   sy-k-R   ,except ['l’amertume'], check the phon for: {'pour': 'puR', 'de': 'd2', 'son': 's§', 'café': 'kafe', 'a': 'a', 'mis': 'mi', 'un': '1', 'sucre': 'sykR'}</t>
+    <t>pu-R   R@-d-R   s§   ka-fe   m-w5   a-mE-R   E-l   a   mi   1   mO-R-so   d2   sy-k-R   ,check the cv for: {'pour': 'puR', 'son': 's§', 'café': 'kafe', 'moins': 'mw5', 'amer': 'amER', 'a': 'a', 'mis': 'mi', 'un': '1', 'de': 'd2', 'sucre': 'sykR'}</t>
   </si>
   <si>
     <t>pu-R   a-me-l-jo-Re   sE-t   i-l   fo-d-RE   a-Zu-te   1   p2   p-ly   d2   sy-k-R   ,except ['recette'], check the phon for: {'pour': 'puR', 'il': 'il', 'un': '1', 'peu': 'p2', 'plus': 'ply', 'de': 'd2', 'sucre': 'sykR'}</t>
   </si>
   <si>
-    <t>Il a mis un couteau sous sa gorge.</t>
-  </si>
-  <si>
-    <t>Elle a encore mal à la gorge.</t>
+    <t>Il lui a mis un couteau sous la gorge.</t>
   </si>
   <si>
     <t>gorge</t>
   </si>
   <si>
-    <t>12, check the cv for: {'il': 2, 'a': 1, 'mis': 1, 'un': 1, 'sous': 1, 'sa': 1, 'gorge': 3}</t>
-  </si>
-  <si>
-    <t>13, check the cv for: {'a': 1, 'mal': 2, 'la': 1, 'gorge': 3}</t>
-  </si>
-  <si>
-    <t>i-l   a   mi   1   ku-to   su   sa   gO-R-Z   ,check the cv for: {'il': 'il', 'a': 'a', 'mis': 'mi', 'un': '1', 'sous': 'su', 'sa': 'sa', 'gorge': 'gORZ'}</t>
-  </si>
-  <si>
-    <t>E-l   a   @-kO-R   ma-l   a   la   gO-R-Z   ,check the cv for: {'a': 'a', 'mal': 'mal', 'la': 'la', 'gorge': 'gORZ'}</t>
+    <t>14, check the cv for: {'il': 2, 'lui': 2, 'a': 1, 'mis': 1, 'un': 1, 'sous': 1, 'la': 1, 'gorge': 3}</t>
+  </si>
+  <si>
+    <t>i-l   l-8i   a   mi   1   ku-to   su   la   gO-R-Z   ,check the cv for: {'il': 'il', 'lui': 'l8i', 'a': 'a', 'mis': 'mi', 'un': '1', 'sous': 'su', 'la': 'la', 'gorge': 'gORZ'}</t>
+  </si>
+  <si>
+    <t>E-l   a   ma-l   a   la   gO-R-Z   ,except ['depuis', "l'accident"], check the phon for: {'a': 'a', 'mal': 'mal', 'la': 'la', 'gorge': 'gORZ'}</t>
   </si>
   <si>
     <t>Bernard l’avait accueilli avec un thé à la menthe.</t>
   </si>
   <si>
-    <t>Isabelle était sortie cueillir un peu de menthe.</t>
+    <t>Isabelle était sortie cueillir un bouquet de menthe.</t>
   </si>
   <si>
     <t>menthe</t>
@@ -304,118 +268,79 @@
     <t>12, except ['bernard', 'l’avait'], check the cv for: {'un': 1, 'la': 1}</t>
   </si>
   <si>
-    <t>18, check the cv for: {'isabelle': 4, 'était': 2, 'sortie': 3, 'un': 1, 'peu': 1, 'de': 1}</t>
+    <t>19, check the cv for: {'isabelle': 4, 'était': 2, 'sortie': 3, 'un': 1, 'de': 1}</t>
   </si>
   <si>
     <t>a-k9-ji   a-vE-k   1   te   a   la   m@-t   ,except ['bernard', 'l’avait'], check the phon for: {'un': '1', 'la': 'la'}</t>
   </si>
   <si>
-    <t>i-za-bE-l   e-tE   sO-R-ti   k9-j-i-R   1   p2   d2   m@-t   ,check the cv for: {'isabelle': 'izabEl', 'était': 'etE', 'sortie': 'sORti', 'un': '1', 'peu': 'p2', 'de': 'd2'}</t>
-  </si>
-  <si>
-    <t>Elle avait pris son nouvel appareil pour prendre de belles photos.</t>
-  </si>
-  <si>
-    <t>La galerie d’art a organisé une belle exposition de photos.</t>
+    <t>i-za-bE-l   e-tE   sO-R-ti   k9-j-i-R   1   bu-kE   d2   m@-t   ,check the cv for: {'isabelle': 'izabEl', 'était': 'etE', 'sortie': 'sORti', 'un': '1', 'de': 'd2'}</t>
+  </si>
+  <si>
+    <t>Elle a emporté son nouvel appareil pour prendre de belles photos.</t>
   </si>
   <si>
     <t>photos</t>
   </si>
   <si>
-    <t>25, check the cv for: {'avait': 2, 'pris': 2, 'son': 1, 'pour': 2, 'de': 1, 'belles': 2}</t>
-  </si>
-  <si>
-    <t>21, except ['galerie', 'd’art'], check the cv for: {'la': 1, 'a': 1, 'organisé': 5, 'une': 2, 'belle': 2, 'de': 1}</t>
-  </si>
-  <si>
-    <t>E-l   a-vE   p-Ri   s§   nu-vE-l   a-pa-RE-j   pu-R   p-R@-d-R   d2   bE-l   fo-to   ,check the cv for: {'avait': 'avE', 'pris': 'pRi', 'son': 's§', 'pour': 'puR', 'de': 'd2', 'belles': 'bEl'}</t>
-  </si>
-  <si>
-    <t>la   a   O-R-ga-ni-ze   y-n   bE-l   E-k-s-po-zi-s-j§   d2   fo-to   ,except ['galerie', 'd’art'], check the phon for: {'la': 'la', 'a': 'a', 'organisé': 'ORganize', 'une': 'yn', 'belle': 'bEl', 'de': 'd2'}</t>
-  </si>
-  <si>
-    <t>Il a encore fait sa tarte aux pommes.</t>
-  </si>
-  <si>
-    <t>Elle a toujours adoré manger des pommes.</t>
+    <t>26, check the cv for: {'a': 1, 'emporté': 4, 'son': 1, 'pour': 2, 'de': 1, 'belles': 2}</t>
+  </si>
+  <si>
+    <t>E-l   a   @-pO-R-te   s§   nu-vE-l   a-pa-RE-j   pu-R   p-R@-d-R   d2   bE-l   fo-to   ,check the cv for: {'a': 'a', 'emporté': '@pORte', 'son': 's§', 'pour': 'puR', 'de': 'd2', 'belles': 'bEl'}</t>
+  </si>
+  <si>
+    <t>s§   pE-R   a   y-n   bE-l   ko-lE-k-s-j§   d2   fo-to   ,check the cv for: {'son': 's§', 'a': 'a', 'une': 'yn', 'belle': 'bEl', 'de': 'd2'}</t>
+  </si>
+  <si>
+    <t>On fait le cidre avec le jus des pommes.</t>
   </si>
   <si>
     <t>pommes</t>
   </si>
   <si>
-    <t>14, check the cv for: {'il': 2, 'a': 1, 'fait': 1, 'sa': 1, 'tarte': 3, 'pommes': 2}</t>
-  </si>
-  <si>
-    <t>14, check the cv for: {'a': 1, 'manger': 2, 'pommes': 2}</t>
-  </si>
-  <si>
-    <t>i-l   a   @-kO-R   fE   sa   ta-R-t   o   pO-m   ,check the cv for: {'il': 'il', 'a': 'a', 'fait': 'fE', 'sa': 'sa', 'tarte': 'taRt', 'pommes': 'pOm'}</t>
+    <t>14, check the cv for: {'on': 1, 'fait': 1, 'le': 1, 'pommes': 2}</t>
+  </si>
+  <si>
+    <t>§   fE   l2   si-d-R   a-vE-k   l2   Zy   de   pO-m   ,check the cv for: {'on': '§', 'fait': 'fE', 'le': 'l2', 'pommes': 'pOm'}</t>
   </si>
   <si>
     <t>E-l   a   tu-Zu-R   a-do-Re   m@-Ze   de   pO-m   ,check the cv for: {'a': 'a', 'manger': 'm@Ze', 'pommes': 'pOm'}</t>
   </si>
   <si>
-    <t>On a appelé les pompiers car le chat était coincé dans l’arbre.</t>
-  </si>
-  <si>
     <t>Nous sommes descendu de la voiture et avons vu un bel arbre.</t>
   </si>
   <si>
     <t>arbre</t>
   </si>
   <si>
-    <t>16, except ['appelé', 'l’arbre'], check the cv for: {'on': 1, 'a': 1, 'les': 1, 'pompiers': 3, 'car': 2, 'le': 1, 'était': 2, 'coincé': 3}</t>
-  </si>
-  <si>
     <t>23, check the cv for: {'sommes': 2, 'de': 1, 'la': 1, 'voiture': 4, 'avons': 2, 'vu': 1, 'un': 1}</t>
   </si>
   <si>
-    <t>§   a   le   p§-p-je   ka-R   l2   Sa   e-tE   k-w5-se   d@   ,except ['appelé', 'l’arbre'], check the phon for: {'on': '§', 'a': 'a', 'les': 'le', 'pompiers': 'p§pje', 'car': 'kaR', 'le': 'l2', 'était': 'etE', 'coincé': 'kw5se'}</t>
+    <t>le   p§-p-je   §   Re-ky-pe-Re   l2   Sa   k-w5-se   @   o   a-R-b-R   ,except ["d'un"], check the phon for: {'les': 'le', 'pompiers': 'p§pje', 'ont': '§', 'le': 'l2', 'coincé': 'kw5se', 'en': '@', 'haut': 'o'}</t>
   </si>
   <si>
     <t>nu   sO-m   de-s@-dy   d2   la   v-wa-ty-R   e   a-v§   vy   1   bE-l   a-R-b-R   ,check the cv for: {'sommes': 'sOm', 'de': 'd2', 'la': 'la', 'voiture': 'vwatyR', 'avons': 'av§', 'vu': 'vy', 'un': '1'}</t>
   </si>
   <si>
-    <t>Si on continue comme ça, on va encore rater notre train.</t>
-  </si>
-  <si>
-    <t>Si elle avait reçu la nouvelle, elle aurait pris le train.</t>
-  </si>
-  <si>
     <t>train</t>
   </si>
   <si>
-    <t>20, check the cv for: {'si': 1, 'on': 1, 'continue': 3, 'comme': 2, 'ça': 1, 'va': 1, 'notre': 3}</t>
-  </si>
-  <si>
-    <t>18, except ['reçu'], check the cv for: {'si': 1, 'avait': 2, 'la': 1, 'nouvelle': 3, 'aurait': 2, 'pris': 2, 'le': 1}</t>
-  </si>
-  <si>
-    <t>si   §   k§-ti-ny   kO-m   sa   §   va   @-kO-R   Ra-te   nO-t-R   t-R5   ,check the cv for: {'si': 'si', 'on': '§', 'continue': 'k§tiny', 'comme': 'kOm', 'ça': 'sa', 'va': 'va', 'notre': 'nOtR'}</t>
-  </si>
-  <si>
-    <t>si   E-l   a-vE   la   nu-vE-l   E-l   o-RE   p-Ri   l2   t-R5   ,except ['reçu'], check the phon for: {'si': 'si', 'avait': 'avE', 'la': 'la', 'nouvelle': 'nuvEl', 'aurait': 'oRE', 'pris': 'pRi', 'le': 'l2'}</t>
-  </si>
-  <si>
-    <t>Au printemps, son père‏ tondait la pelouse.</t>
-  </si>
-  <si>
-    <t>En été, les enfants jouaient sur la pelouse.</t>
+    <t>22, except [''], check the cv for: {'la': 1, 'gare': 2, 'est': 1, 'de': 1, 'notre': 3}</t>
+  </si>
+  <si>
+    <t>la   ga-R   e   @-kO-R   l-w5   e   nu   Ri-s-k§   d2   Ra-te   nO-t-R   t-R5   ,except [''], check the phon for: {'la': 'la', 'gare': 'gaR', 'est': 'e', 'de': 'd2', 'notre': 'nOtR'}</t>
+  </si>
+  <si>
+    <t>nu   a-v§   fi-ni   no   E-g-za-m5   e   nu   vu-d-Ri-j§   p-R@-d-R   nO-t-R   t-R5   ,check the cv for: {'avons': 'av§', 'fini': 'fini', 'notre': 'nOtR'}</t>
   </si>
   <si>
     <t>pelouse</t>
   </si>
   <si>
-    <t>8, except ['père\u200f', 'pelouse'], check the cv for: {'son': 1, 'la': 1}</t>
-  </si>
-  <si>
-    <t>11, except ['pelouse'], check the cv for: {'en': 1, 'été': 2, 'les': 1, 'sur': 2, 'la': 1}</t>
-  </si>
-  <si>
-    <t>o   p-R5-t@   s§   t§-dE   la   ,except ['père\u200f', 'pelouse'], check the phon for: {'son': 's§', 'la': 'la'}</t>
-  </si>
-  <si>
-    <t>@   e-te   le   @-f@   Z-wE   sy-R   la   ,except ['pelouse'], check the phon for: {'en': '@', 'été': 'ete', 'les': 'le', 'sur': 'syR', 'la': 'la'}</t>
+    <t>o   p-R5-t@   d@   l2   Za-R-d5   s§   t§-dE   la   ,except ['père\u200f', 'pelouse'], check the phon for: {'le': 'l2', 'son': 's§', 'la': 'la'}</t>
+  </si>
+  <si>
+    <t>@   e-te   o   bO-R   d2   la   mE-R   le   @-f@   Z-wE   sy-R   la   ,except ['pelouse'], check the phon for: {'en': '@', 'été': 'ete', 'de': 'd2', 'la': 'la', 'les': 'le', 'sur': 'syR'}</t>
   </si>
   <si>
     <t>Dès sa majorité, il s’était engagé dans l’armée.</t>
@@ -451,76 +376,34 @@
     <t>18, check the cv for: {'après': 3, 'grosse': 3, 'il': 2, 'de': 1}</t>
   </si>
   <si>
-    <t>15, except ["l'après"], check the cv for: {'midi': 2, 'il': 2, 'su': 1, 'pourquoi': 4, 'avait': 2}</t>
-  </si>
-  <si>
     <t>a-p-RE   sE-t   g-Ro-s   be-ti-z   i-l   Ru-Zi   d2   §-t   ,check the cv for: {'après': 'apRE', 'grosse': 'gRos', 'il': 'il', 'de': 'd2'}</t>
   </si>
   <si>
     <t>mi-di   i-l   sy   pu-R-k-wa   i-l   a-vE   §-t   ,except ["l'après"], check the phon for: {'midi': 'midi', 'il': 'il', 'su': 'sy', 'pourquoi': 'puRkwa', 'avait': 'avE'}</t>
   </si>
   <si>
-    <t>Ces pommes rouges ont très bon goût</t>
-  </si>
-  <si>
-    <t>Ces vieux hommes ont très mauvais goût</t>
-  </si>
-  <si>
-    <t>goût</t>
-  </si>
-  <si>
-    <t>10, check the cv for: {'pommes': 2, 'rouges': 2, 'ont': 1, 'bon': 1}</t>
-  </si>
-  <si>
-    <t>11, check the cv for: {'vieux': 2, 'ont': 1, 'mauvais': 2}</t>
-  </si>
-  <si>
-    <t>se   pO-m   Ru-Z   §   t-RE   b§   gu   ,check the cv for: {'pommes': 'pOm', 'rouges': 'RuZ', 'ont': '§', 'bon': 'b§'}</t>
-  </si>
-  <si>
-    <t>se   v-j2   O-m   §   t-RE   mo-vE   gu   ,check the cv for: {'vieux': 'vj2', 'ont': '§', 'mauvais': 'movE'}</t>
-  </si>
-  <si>
-    <t>Les gentils garçons l'aident à pousser sa voiture</t>
-  </si>
-  <si>
-    <t>Elle a voulu réparer sa propre voiture</t>
+    <t>Après sa panne, un passant l'a aidé à pousser sa voiture</t>
+  </si>
+  <si>
+    <t>Comme ses voisins, elle a elle-même repeint sa voiture</t>
   </si>
   <si>
     <t>voiture</t>
   </si>
   <si>
-    <t>14, except ["l'aident"], check the cv for: {'les': 1, 'gentils': 2, 'sa': 1, 'voiture': 4}</t>
-  </si>
-  <si>
-    <t>17, check the cv for: {'a': 1, 'voulu': 2, 'sa': 1, 'propre': 4, 'voiture': 4}</t>
-  </si>
-  <si>
-    <t>le   Z@-ti   ga-R-s§   a   pu-se   sa   v-wa-ty-R   ,except ["l'aident"], check the phon for: {'les': 'le', 'gentils': 'Z@ti', 'sa': 'sa', 'voiture': 'vwatyR'}</t>
-  </si>
-  <si>
-    <t>E-l   a   vu-ly   Re-pa-Re   sa   p-RO-p-R   v-wa-ty-R   ,check the cv for: {'a': 'a', 'voulu': 'vuly', 'sa': 'sa', 'propre': 'pROpR', 'voiture': 'vwatyR'}</t>
-  </si>
-  <si>
-    <t>Finalement, elle a dit qu'il n'y a rien comme vivre à la campagne.</t>
-  </si>
-  <si>
-    <t>Après quelques jours, il a dit qu'il voulait retourner dans sa campagne</t>
+    <t>a-p-RE   sa   pa-n   1   pa-s@   E-de   a   pu-se   sa   v-wa-ty-R   ,except ["l'a"], check the phon for: {'après': 'apRE', 'sa': 'sa', 'un': '1', 'passant': 'pas@', 'voiture': 'vwatyR'}</t>
+  </si>
+  <si>
+    <t>kO-m   se   v-wa-z5   E-l   a   E-l   mE-m   sa   v-wa-ty-R   ,except ['repeint'], check the phon for: {'comme': 'kOm', 'ses': 'se', 'voisins': 'vwaz5', 'a': 'a', 'même': 'mEm', 'sa': 'sa', 'voiture': 'vwatyR'}</t>
   </si>
   <si>
     <t>campagne</t>
   </si>
   <si>
-    <t>17, except ['finalement', "qu'il", "n'y"], check the cv for: {'a': 1, 'dit': 1, 'rien': 2, 'comme': 2, 'vivre': 3, 'la': 1}</t>
-  </si>
-  <si>
-    <t>19, except ["qu'il", 'retourner'], check the cv for: {'après': 3, 'il': 2, 'a': 1, 'dit': 1, 'sa': 1}</t>
-  </si>
-  <si>
-    <t>E-l   a   di   a   R-j5   kO-m   vi-v-R   a   la   k@-pa-N   ,except ['finalement', "qu'il", "n'y"], check the phon for: {'a': 'a', 'dit': 'di', 'rien': 'Rj5', 'comme': 'kOm', 'vivre': 'vivR', 'la': 'la'}</t>
-  </si>
-  <si>
-    <t>a-p-RE   kE-l-k   Zu-R   i-l   a   di   vu-lE   d@   sa   k@-pa-N   ,except ["qu'il", 'retourner'], check the phon for: {'après': 'apRE', 'il': 'il', 'a': 'a', 'dit': 'di', 'sa': 'sa'}</t>
+    <t>d@   y-n   fE-R-m   i-l   RE-v   d2   vi-v-R   d@   la   k@-pa-N   ,except ['elevé', 'retourner'], check the phon for: {'une': 'yn', 'ferme': 'fERm', 'il': 'il', 'rêve': 'REv', 'de': 'd2', 'vivre': 'vivR', 'la': 'la'}</t>
+  </si>
+  <si>
+    <t>a   la   f5   de   va-k@-s   i-l   a   de-si-de   d2   d@   la   k@-pa-N   ,except ['retourner'], check the phon for: {'a': 'a', 'la': 'la', 'fin': 'f5', 'il': 'il', 'décidé': 'deside', 'de': 'd2'}</t>
   </si>
   <si>
     <t>Elle aime ce film sans en comprendre le sens</t>
@@ -535,41 +418,167 @@
     <t>17, check the cv for: {'ce': 1, 'en': 1, 'le': 1, 'sens': 1}</t>
   </si>
   <si>
-    <t>13, except ['georges'], check the cv for: {'que': 1, 'a': 1, 'un': 1, 'sens': 1}</t>
-  </si>
-  <si>
     <t>E-l   E-m   s2   fi-l-m   s@   @   k§-p-R@-d-R   l2   s@   ,check the cv for: {'ce': 's2', 'en': '@', 'le': 'l2', 'sens': 's@'}</t>
   </si>
   <si>
     <t>p@-s   k2   sE-t   i-s-t-wa-R   a   1   s@   ,except ['georges'], check the phon for: {'que': 'k2', 'a': 'a', 'un': '1', 'sens': 's@'}</t>
   </si>
   <si>
-    <t>Il décida de vendre ses actions en bourse</t>
-  </si>
-  <si>
-    <t>Elle n'a presque jamais affaire à la bourse</t>
+    <t>Il va acheter des actions cotées en bourse</t>
   </si>
   <si>
     <t>bourse</t>
   </si>
   <si>
-    <t>18, check the cv for: {'il': 2, 'de': 1, 'ses': 1, 'actions': 4, 'en': 1}</t>
-  </si>
-  <si>
-    <t>16, except ["n'a"], check the cv for: {'affaire': 3, 'la': 1}</t>
-  </si>
-  <si>
-    <t>i-l   de-si-da   d2   v@-d-R   se   a-k-s-j§   @   bu-R-s   ,check the cv for: {'il': 'il', 'de': 'd2', 'ses': 'se', 'actions': 'aksj§', 'en': '@'}</t>
-  </si>
-  <si>
-    <t>E-l   p-RE-s-k   Za-mE   a-fE-R   a   la   bu-R-s   ,except ["n'a"], check the phon for: {'affaire': 'afER', 'la': 'la'}</t>
+    <t>i-l   va   de   a-k-s-j§   ko-te   @   bu-R-s   ,except ['acheter'], check the phon for: {'il': 'il', 'va': 'va', 'actions': 'aksj§', 'cotées': 'kote', 'en': '@'}</t>
+  </si>
+  <si>
+    <t>E-l   Za-mE   pa-se   la   bu-R-s   ,except ["n'est", 'devant'], check the phon for: {'passée': 'pase', 'la': 'la'}</t>
+  </si>
+  <si>
+    <t>Il aime le commerce et a décidé d'ouvrir un magasin de lunettes.</t>
+  </si>
+  <si>
+    <t>lunettes</t>
+  </si>
+  <si>
+    <t>sa   vy   a   be-se   e   i-l   d-wa   y-n   nu-vE-l   pE-R   d2   ly-nE-t   ,except ['acheter'], check the phon for: {'sa': 'sa', 'vue': 'vy', 'a': 'a', 'il': 'il', 'doit': 'dwa', 'une': 'yn', 'nouvelle': 'nuvEl', 'paire': 'pER', 'de': 'd2'}</t>
+  </si>
+  <si>
+    <t>i-l   E-m   l2   ko-mE-R-s   e   a   de-si-de   1   ma-ga-z5   d2   ly-nE-t   ,except ["d'ouvrir"], check the phon for: {'il': 'il', 'le': 'l2', 'commerce': 'komERs', 'a': 'a', 'décidé': 'deside', 'un': '1', 'de': 'd2'}</t>
+  </si>
+  <si>
+    <t>fourchette</t>
+  </si>
+  <si>
+    <t>l2   ga-R-s§   m@-Z   s§   bi-f-tE-k   a-vE-k   1   ku-to   e   y-n   fu-R-SE-t   ,except ['petit'], check the phon for: {'le': 'l2', 'son': 's§', 'un': '1', 'une': 'yn'}</t>
+  </si>
+  <si>
+    <t>la   v-jE-j   fa-m   mE   d@   s§   sa-k   1   b-Ri-kE   e   y-n   fu-R-SE-t   ,check the cv for: {'la': 'la', 'vieille': 'vjEj', 'son': 's§', 'un': '1', 'une': 'yn'}</t>
+  </si>
+  <si>
+    <t>usé</t>
+  </si>
+  <si>
+    <t>Les visiteurs attendaient le maire et pensaient qu'il avait disparu.</t>
+  </si>
+  <si>
+    <t>Pour améliorer cette recette, il faudrait ajouter un peu de sucre.</t>
+  </si>
+  <si>
+    <t>En été à la mer, les enfants jouaient sur la pelouse.</t>
+  </si>
+  <si>
+    <t>18, check the cv for: {'le': 1, 'son': 1, 'la': 1}</t>
+  </si>
+  <si>
+    <t>19, check the cv for: {'en': 1, 'été': 2, 'de': 1, 'la': 1, 'les': 1, 'sur': 2}</t>
+  </si>
+  <si>
+    <t>20, check the cv for: {'après': 3, 'sa': 1, 'un': 1, 'passant': 2, 'voiture': 4}</t>
+  </si>
+  <si>
+    <t>18, check the cv for: {'midi': 2, 'il': 2, 'su': 1, 'pourquoi': 4, 'avait': 2}</t>
+  </si>
+  <si>
+    <t>20, check the cv for: {'comme': 2, 'ses': 1, 'voisins': 3, 'a': 1, 'même': 2, 'sa': 1, 'voiture': 4}</t>
+  </si>
+  <si>
+    <t>26, check the cv for: {'une': 2, 'ferme': 3, 'il': 2, 'rêve': 2, 'de': 1, 'vivre': 3, 'la': 1}</t>
+  </si>
+  <si>
+    <t>16, check the cv for: {'que': 1, 'a': 1, 'un': 1, 'sens': 1}</t>
+  </si>
+  <si>
+    <t>Dès la première goutte de pluie elle a ouvert son parapluie.</t>
+  </si>
+  <si>
+    <t>17 check the cv for: {'il': 2, 'va': 1, 'actions': 4, 'cotées': 2, 'en': 1}</t>
+  </si>
+  <si>
+    <t>Elle n'est encore jamais passée devant la bourse</t>
+  </si>
+  <si>
+    <t>16, check the cv for: {'passée': 2, 'la': 1}</t>
+  </si>
+  <si>
+    <t>26, check the cv for: {'il': 2, 'le': 1, 'commerce': 4, 'a': 1, 'décidé': 3, 'un': 1, 'de': 1}</t>
+  </si>
+  <si>
+    <t>La vieille femme met dans son sac un petit briquet et une fourchette.</t>
+  </si>
+  <si>
+    <t>24, check the cv for: {'la': 1, 'vieille': 3, 'son': 1, 'un': 1, 'une': 2}</t>
+  </si>
+  <si>
+    <t>Le petit garçon mange son steak avec un couteau et une fourchette.</t>
+  </si>
+  <si>
+    <t>25, check the cv for: {'le': 1, 'son': 1, 'un': 1, 'une': 2}</t>
+  </si>
+  <si>
+    <t>parapluie</t>
+  </si>
+  <si>
+    <t>Elle a toujours eu mal à la gorge.</t>
+  </si>
+  <si>
+    <t>14, check the cv for: {'a': 1, 'mal': 2, 'la': 1, 'gorge': 3}</t>
+  </si>
+  <si>
+    <t>Les pompiers ont enfin récupéré le chat coincé en haut d'un arbre.</t>
+  </si>
+  <si>
+    <t>23, check the cv for: {'les': 1, 'pompiers': 3, 'ont': 1, 'le': 1, 'coincé': 3, 'en': 1, 'haut': 1}</t>
+  </si>
+  <si>
+    <t>26, check the cv for: {'sa': 1, 'vue': 1, 'a': 1, 'il': 2, 'doit': 2, 'une': 2, 'nouvelle': 3, 'paire': 2, 'de': 1}</t>
+  </si>
+  <si>
+    <t>Son père avait dans le temps une incroyable collection de photos.</t>
+  </si>
+  <si>
+    <t>25, check the cv for: {'son': 1, 'a': 1, 'une': 2, 'belle': 2, 'de': 1}</t>
+  </si>
+  <si>
+    <t>Son ami a toujours adoré manger des pommes.</t>
+  </si>
+  <si>
+    <t>15, check the cv for: {'a': 1, 'manger': 2, 'pommes': 2}</t>
+  </si>
+  <si>
+    <t>Au printemps dans le jardin, son père tondait la pelouse.</t>
+  </si>
+  <si>
+    <t>La gare est encore très loin, et nous allons rater notre train.</t>
+  </si>
+  <si>
+    <t>23, check the cv for: {'avons': 2, 'fini': 2, 'notre': 3}</t>
+  </si>
+  <si>
+    <t>Elevé dans une ferme, il rêve de retourner vivre à la campagne.</t>
+  </si>
+  <si>
+    <t>A la fin des vacances, Eloïse décida de retourner dans la campagne.</t>
+  </si>
+  <si>
+    <t>25, check the cv for: {'a': 1, 'la': 1, 'fin': 1, 'il': 2, 'décidé': 3, 'de': 1}</t>
+  </si>
+  <si>
+    <t>Dès son arrivée dans le grand magasin elle s'est acheté un parapluie.</t>
+  </si>
+  <si>
+    <t>Nous avons enfin fini nos examens, et nous allons prendre le train.</t>
+  </si>
+  <si>
+    <t>Sa vue a diminué et elle doit acheter une nouvelle paire de lunettes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +709,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1046,52 +1062,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1107,7 +1126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1402,15 +1421,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1450,8 +1476,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -1491,8 +1517,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
@@ -1502,7 +1528,7 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -1520,7 +1546,7 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1532,320 +1558,320 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
       <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
         <v>32</v>
       </c>
-      <c r="M4" t="s">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>59</v>
+      </c>
+      <c r="H5" t="s">
         <v>36</v>
       </c>
-      <c r="D5">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5">
-        <v>54</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
       <c r="I5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5">
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M5" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
         <v>44</v>
       </c>
-      <c r="F6">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>-3</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7">
-        <v>66</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7">
-        <v>14</v>
-      </c>
-      <c r="G7">
+      <c r="H8" t="s">
         <v>57</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7">
-        <v>14</v>
-      </c>
-      <c r="J7">
-        <v>9</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>59</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>-2</v>
+      </c>
+      <c r="K9">
         <v>-1</v>
       </c>
-      <c r="K8">
-        <v>-1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>60</v>
-      </c>
-      <c r="M8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="L9" t="s">
         <v>65</v>
       </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="M9" t="s">
         <v>66</v>
       </c>
-      <c r="I9">
-        <v>10</v>
-      </c>
-      <c r="J9">
-        <v>7</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M9" t="s">
+      <c r="B10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" t="s">
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>-8</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
         <v>71</v>
       </c>
-      <c r="D10">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="M10" t="s">
         <v>72</v>
       </c>
-      <c r="F10">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I11">
         <v>8</v>
-      </c>
-      <c r="G10">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10">
-        <v>9</v>
-      </c>
-      <c r="J10">
-        <v>-2</v>
-      </c>
-      <c r="K10">
-        <v>-1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>74</v>
-      </c>
-      <c r="M10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11">
-        <v>55</v>
-      </c>
-      <c r="E11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11">
-        <v>12</v>
       </c>
       <c r="J11">
         <v>-3</v>
@@ -1854,585 +1880,611 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
         <v>81</v>
       </c>
-      <c r="M11" t="s">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12">
+      <c r="I12">
         <v>8</v>
       </c>
-      <c r="G12">
-        <v>22</v>
-      </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
       <c r="J12">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D13">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G13">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>172</v>
       </c>
       <c r="I13">
         <v>8</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D14">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>174</v>
       </c>
       <c r="I14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J14">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="M14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>104</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D15">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G15">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="I15">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J15">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="M15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>111</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D16">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G16">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="I16">
         <v>12</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D17">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="F17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="I17">
         <v>11</v>
       </c>
       <c r="J17">
+        <v>-1</v>
+      </c>
+      <c r="K17">
         <v>-2</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
       <c r="L17" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="M17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>125</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="D18">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18">
         <v>7</v>
       </c>
-      <c r="G18">
-        <v>35</v>
-      </c>
-      <c r="H18" t="s">
-        <v>129</v>
-      </c>
-      <c r="I18">
-        <v>8</v>
-      </c>
       <c r="J18">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K18">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="M18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>132</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D19">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F19">
         <v>8</v>
       </c>
       <c r="G19">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="I19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>118</v>
+      </c>
+      <c r="M19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>123</v>
+      </c>
+      <c r="M20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>51</v>
+      </c>
+      <c r="H21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I21">
+        <v>13</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
         <v>-1</v>
       </c>
-      <c r="K19">
+      <c r="L21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>155</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22">
         <v>1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>137</v>
-      </c>
-      <c r="M19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D20">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
-      </c>
-      <c r="G20">
-        <v>36</v>
-      </c>
-      <c r="H20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I20">
-        <v>8</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>144</v>
-      </c>
-      <c r="M20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21">
-        <v>29</v>
-      </c>
-      <c r="E21" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>32</v>
-      </c>
-      <c r="H21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I21">
-        <v>7</v>
-      </c>
-      <c r="J21">
-        <v>-3</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>151</v>
-      </c>
-      <c r="M21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>156</v>
-      </c>
-      <c r="F22">
-        <v>8</v>
-      </c>
-      <c r="G22">
-        <v>32</v>
-      </c>
-      <c r="H22" t="s">
-        <v>157</v>
-      </c>
-      <c r="I22">
-        <v>7</v>
-      </c>
-      <c r="J22">
-        <v>10</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
       <c r="L22" t="s">
+        <v>132</v>
+      </c>
+      <c r="M22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
         <v>158</v>
       </c>
-      <c r="M22" t="s">
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="I23">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>136</v>
+      </c>
+      <c r="M23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="1">
+        <v>53</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" s="1">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1">
+        <v>52</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B23" t="s">
+      <c r="I24" s="1">
+        <v>12</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" t="s">
         <v>161</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25">
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <v>51</v>
+      </c>
+      <c r="H25" t="s">
         <v>162</v>
       </c>
-      <c r="D23">
-        <v>52</v>
-      </c>
-      <c r="E23" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23">
+      <c r="I25">
         <v>13</v>
       </c>
-      <c r="G23">
-        <v>59</v>
-      </c>
-      <c r="H23" t="s">
-        <v>164</v>
-      </c>
-      <c r="I23">
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>143</v>
+      </c>
+      <c r="M25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="I26">
         <v>12</v>
       </c>
-      <c r="J23">
-        <v>-7</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
-        <v>165</v>
-      </c>
-      <c r="M23" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24" t="s">
-        <v>168</v>
-      </c>
-      <c r="C24" t="s">
-        <v>169</v>
-      </c>
-      <c r="D24">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>170</v>
-      </c>
-      <c r="F24">
-        <v>9</v>
-      </c>
-      <c r="G24">
-        <v>35</v>
-      </c>
-      <c r="H24" t="s">
-        <v>171</v>
-      </c>
-      <c r="I24">
-        <v>8</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>172</v>
-      </c>
-      <c r="M24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" t="s">
-        <v>176</v>
-      </c>
-      <c r="D25">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
-        <v>177</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
-      </c>
-      <c r="G25">
-        <v>36</v>
-      </c>
-      <c r="H25" t="s">
-        <v>178</v>
-      </c>
-      <c r="I25">
-        <v>8</v>
-      </c>
-      <c r="J25">
-        <v>-2</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>179</v>
-      </c>
-      <c r="M25" t="s">
-        <v>180</v>
-      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>